<commit_message>
Correcçâo Diagrama Casos de Uso
1 hora para o mapa de horas
</commit_message>
<xml_diff>
--- a/DOC/Engenharia Software II/Mapa de horas.xlsx
+++ b/DOC/Engenharia Software II/Mapa de horas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\checonight\Desktop\eng sot2 2017\trabalho final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\checonight\Desktop\eng sot2 2017\gitub\ProgramacaoInternet\DOC\Engenharia Software II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>André Madeira</t>
   </si>
@@ -256,13 +256,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -274,14 +271,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90DF40B-70A9-4F47-9831-A191BA050E06}">
   <dimension ref="A2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,89 +625,89 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12" t="s">
+      <c r="L6" s="15"/>
+      <c r="M6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
@@ -894,36 +894,36 @@
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12" t="s">
+      <c r="H12" s="15"/>
+      <c r="I12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12" t="s">
+      <c r="J12" s="15"/>
+      <c r="K12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12" t="s">
+      <c r="L12" s="15"/>
+      <c r="M12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="12"/>
+      <c r="N12" s="15"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
@@ -979,8 +979,12 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1006,8 +1010,12 @@
       <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1033,8 +1041,12 @@
       <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1062,36 +1074,36 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12" t="s">
+      <c r="H18" s="15"/>
+      <c r="I18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12" t="s">
+      <c r="J18" s="15"/>
+      <c r="K18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12" t="s">
+      <c r="L18" s="15"/>
+      <c r="M18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="12"/>
+      <c r="N18" s="15"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
@@ -1264,227 +1276,269 @@
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="18" t="s">
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="14"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="18" t="s">
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="15"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="18" t="s">
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="15"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="14"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="18" t="s">
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="15"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="14"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="18" t="s">
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="15"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="14"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="18" t="s">
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="15"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="14"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="18" t="s">
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="15"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="14"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="18" t="s">
+      <c r="C36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="15"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="14"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="18" t="s">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="18"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="18" t="s">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I38" s="18"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="18" t="s">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I39" s="18"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="B2:N4"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="J36:N36"/>
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="J38:N38"/>
     <mergeCell ref="J39:N39"/>
@@ -1501,46 +1555,6 @@
     <mergeCell ref="J34:N34"/>
     <mergeCell ref="J35:N35"/>
     <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="J36:N36"/>
-    <mergeCell ref="J37:N37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="B2:N4"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update mapa de horas
update descrição casos de uso
</commit_message>
<xml_diff>
--- a/DOC/Engenharia Software II/Mapa de horas.xlsx
+++ b/DOC/Engenharia Software II/Mapa de horas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\checonight\Desktop\eng sot2 2017\gitub\ProgramacaoInternet\DOC\Engenharia Software II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\checonight\Desktop\eng sot2 2017\trabalho final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
   <si>
     <t>André Madeira</t>
   </si>
@@ -130,6 +130,21 @@
   </si>
   <si>
     <t>Alteraçoes Diagrama de Casos de Uso</t>
+  </si>
+  <si>
+    <t>Diagrama Casos de Uso update</t>
+  </si>
+  <si>
+    <t>diagrama de classes</t>
+  </si>
+  <si>
+    <t>diagrama de classes update</t>
+  </si>
+  <si>
+    <t>diagram de Sequencia "criar trilho"</t>
+  </si>
+  <si>
+    <t>ER</t>
   </si>
 </sst>
 </file>
@@ -599,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90DF40B-70A9-4F47-9831-A191BA050E06}">
   <dimension ref="A2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,17 +995,29 @@
         <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>4</v>
+      </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
@@ -1011,17 +1038,29 @@
         <v>1</v>
       </c>
       <c r="G15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>4</v>
+      </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
@@ -1042,17 +1081,29 @@
         <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>2</v>
+      </c>
+      <c r="N16" s="2">
+        <v>4</v>
+      </c>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
@@ -1147,14 +1198,30 @@
       <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>4</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1166,14 +1233,30 @@
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>4</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1185,14 +1268,30 @@
       <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1287,11 +1386,13 @@
         <v>23</v>
       </c>
       <c r="I29" s="10"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="14"/>
+      <c r="J29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
@@ -1308,7 +1409,9 @@
         <v>24</v>
       </c>
       <c r="I30" s="10"/>
-      <c r="J30" s="12"/>
+      <c r="J30" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
@@ -1329,7 +1432,9 @@
         <v>25</v>
       </c>
       <c r="I31" s="10"/>
-      <c r="J31" s="12"/>
+      <c r="J31" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
@@ -1350,7 +1455,9 @@
         <v>26</v>
       </c>
       <c r="I32" s="10"/>
-      <c r="J32" s="12"/>
+      <c r="J32" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
@@ -1444,11 +1551,13 @@
       <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="C37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="14"/>
       <c r="H37" s="10" t="s">
         <v>31</v>
       </c>
@@ -1463,11 +1572,13 @@
       <c r="B38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="C38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
       <c r="H38" s="10" t="s">
         <v>32</v>
       </c>
@@ -1482,7 +1593,9 @@
       <c r="B39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>

</xml_diff>

<commit_message>
UPDATE DIAGRAMA DE CLASSES E SEQUENCIA e mapa de horas
</commit_message>
<xml_diff>
--- a/DOC/Engenharia Software II/Mapa de horas.xlsx
+++ b/DOC/Engenharia Software II/Mapa de horas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
   <si>
     <t>André Madeira</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>ER</t>
+  </si>
+  <si>
+    <t>diagrama classes e sequencia update</t>
   </si>
 </sst>
 </file>
@@ -271,10 +274,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -286,17 +292,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,7 +618,7 @@
   <dimension ref="A2:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,89 +643,89 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15" t="s">
+      <c r="J6" s="12"/>
+      <c r="K6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15" t="s">
+      <c r="L6" s="12"/>
+      <c r="M6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
@@ -909,36 +912,36 @@
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15" t="s">
+      <c r="J12" s="12"/>
+      <c r="K12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15" t="s">
+      <c r="L12" s="12"/>
+      <c r="M12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="15"/>
+      <c r="N12" s="12"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
@@ -1125,36 +1128,36 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="15" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15" t="s">
+      <c r="H18" s="12"/>
+      <c r="I18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15" t="s">
+      <c r="J18" s="12"/>
+      <c r="K18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15" t="s">
+      <c r="L18" s="12"/>
+      <c r="M18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="12"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
@@ -1222,8 +1225,12 @@
       <c r="J20" s="2">
         <v>2</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="5"/>
@@ -1257,8 +1264,12 @@
       <c r="J21" s="2">
         <v>2</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="5"/>
@@ -1292,8 +1303,12 @@
       <c r="J22" s="2">
         <v>2</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="5"/>
@@ -1375,262 +1390,261 @@
       <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="10" t="s">
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="11" t="s">
+      <c r="I29" s="16"/>
+      <c r="J29" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="10" t="s">
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="12" t="s">
+      <c r="I30" s="16"/>
+      <c r="J30" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="10" t="s">
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="12" t="s">
+      <c r="I31" s="16"/>
+      <c r="J31" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="15"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="10" t="s">
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="12" t="s">
+      <c r="I32" s="16"/>
+      <c r="J32" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="15"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="10" t="s">
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="14"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="15"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="10" t="s">
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="10"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="14"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="15"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="10" t="s">
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="14"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="15"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="10" t="s">
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="14"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="15"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="10" t="s">
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="10" t="s">
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="10" t="s">
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="J36:N36"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J38:N38"/>
+    <mergeCell ref="J39:N39"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J33:N33"/>
     <mergeCell ref="J37:N37"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="J29:N29"/>
@@ -1647,27 +1661,30 @@
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="J36:N36"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J38:N38"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J33:N33"/>
     <mergeCell ref="J34:N34"/>
     <mergeCell ref="J35:N35"/>
     <mergeCell ref="H35:I35"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>